<commit_message>
adding the entry function and exit function and generating ticket id with random function
</commit_message>
<xml_diff>
--- a/03 Banking System Simulation/accounts/saving/254695.xlsx
+++ b/03 Banking System Simulation/accounts/saving/254695.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>NAME</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>13-01-2026 20:29:11</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>aditya dagar</t>
@@ -82,7 +79,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -101,27 +98,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -150,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,28 +140,22 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -490,17 +466,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -531,47 +507,43 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="4">
+        <v>254695</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1341321</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>7015</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6">
-        <v>254695</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1341321</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>7015</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="K2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>